<commit_message>
lista tarefas publicadas e por publicasr
</commit_message>
<xml_diff>
--- a/BaseDados/Dados BD.xlsx
+++ b/BaseDados/Dados BD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blest\Desktop\Sprints\upskill_java1_labprg_grupo2\BaseDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAC960A-4531-4007-98D1-DDA249FBFE88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E7B45C-1CA2-4378-B03A-8B193497F94A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="480" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{657CB9A2-C43B-426B-A736-BB7BF31CC9FD}"/>
+    <workbookView xWindow="28680" yWindow="480" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{657CB9A2-C43B-426B-A736-BB7BF31CC9FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Organização_BD" sheetId="7" r:id="rId1"/>
@@ -2906,7 +2906,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -3761,7 +3761,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4115,6 +4115,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4172,22 +4187,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
@@ -4202,31 +4220,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4579,16 +4582,16 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="121" t="s">
+      <c r="H4" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="121"/>
-      <c r="J4" s="121"/>
-      <c r="K4" s="121"/>
-      <c r="L4" s="121" t="s">
+      <c r="I4" s="126"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="126"/>
+      <c r="L4" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="121"/>
+      <c r="M4" s="126"/>
       <c r="N4" s="1"/>
       <c r="O4" t="s">
         <v>897</v>
@@ -4721,11 +4724,11 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F10" s="122" t="s">
+      <c r="F10" s="127" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="122"/>
-      <c r="H10" s="122"/>
+      <c r="G10" s="127"/>
+      <c r="H10" s="127"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -4981,13 +4984,13 @@
   <sheetData>
     <row r="3" spans="2:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
-      <c r="C3" s="123" t="s">
+      <c r="C3" s="128" t="s">
         <v>588</v>
       </c>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
     </row>
     <row r="4" spans="2:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
@@ -5004,12 +5007,12 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="121" t="s">
+      <c r="H5" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="121"/>
-      <c r="J5" s="121"/>
-      <c r="K5" s="121"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="126"/>
+      <c r="K5" s="126"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
@@ -6277,13 +6280,13 @@
     </row>
     <row r="45" spans="2:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B45" s="3"/>
-      <c r="C45" s="123" t="s">
+      <c r="C45" s="128" t="s">
         <v>625</v>
       </c>
-      <c r="D45" s="123"/>
-      <c r="E45" s="123"/>
-      <c r="F45" s="123"/>
-      <c r="G45" s="123"/>
+      <c r="D45" s="128"/>
+      <c r="E45" s="128"/>
+      <c r="F45" s="128"/>
+      <c r="G45" s="128"/>
     </row>
     <row r="46" spans="2:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B46" s="3"/>
@@ -6325,7 +6328,7 @@
       <c r="B49" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="C49" s="154" t="s">
+      <c r="C49" s="159" t="s">
         <v>728</v>
       </c>
       <c r="D49" s="40" t="s">
@@ -6345,7 +6348,7 @@
       <c r="B50" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="C50" s="154"/>
+      <c r="C50" s="159"/>
       <c r="D50" s="40" t="s">
         <v>643</v>
       </c>
@@ -6703,7 +6706,7 @@
       <c r="B68" s="40" t="s">
         <v>817</v>
       </c>
-      <c r="C68" s="154" t="s">
+      <c r="C68" s="159" t="s">
         <v>632</v>
       </c>
       <c r="D68" s="40" t="s">
@@ -6723,7 +6726,7 @@
       <c r="B69" s="40" t="s">
         <v>818</v>
       </c>
-      <c r="C69" s="154"/>
+      <c r="C69" s="159"/>
       <c r="D69" s="40" t="s">
         <v>645</v>
       </c>
@@ -6801,7 +6804,7 @@
       <c r="B73" s="40" t="s">
         <v>815</v>
       </c>
-      <c r="C73" s="154" t="s">
+      <c r="C73" s="159" t="s">
         <v>627</v>
       </c>
       <c r="D73" s="40" t="s">
@@ -6821,7 +6824,7 @@
       <c r="B74" s="40" t="s">
         <v>816</v>
       </c>
-      <c r="C74" s="154"/>
+      <c r="C74" s="159"/>
       <c r="D74" s="40" t="s">
         <v>644</v>
       </c>
@@ -6897,13 +6900,13 @@
     </row>
     <row r="81" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B81" s="3"/>
-      <c r="C81" s="123" t="s">
+      <c r="C81" s="128" t="s">
         <v>664</v>
       </c>
-      <c r="D81" s="123"/>
-      <c r="E81" s="123"/>
-      <c r="F81" s="123"/>
-      <c r="G81" s="123"/>
+      <c r="D81" s="128"/>
+      <c r="E81" s="128"/>
+      <c r="F81" s="128"/>
+      <c r="G81" s="128"/>
     </row>
     <row r="82" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B82" s="3"/>
@@ -6942,7 +6945,7 @@
       <c r="B85" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C85" s="146" t="s">
+      <c r="C85" s="152" t="s">
         <v>626</v>
       </c>
       <c r="D85" s="5" t="s">
@@ -6957,7 +6960,7 @@
       <c r="B86" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C86" s="148"/>
+      <c r="C86" s="154"/>
       <c r="D86" s="10" t="s">
         <v>374</v>
       </c>
@@ -7098,7 +7101,7 @@
       <c r="B105" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C105" s="147" t="s">
+      <c r="C105" s="153" t="s">
         <v>627</v>
       </c>
       <c r="D105" s="54" t="s">
@@ -7113,7 +7116,7 @@
       <c r="B106" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="C106" s="148"/>
+      <c r="C106" s="154"/>
       <c r="D106" s="10" t="s">
         <v>266</v>
       </c>
@@ -7126,7 +7129,7 @@
       <c r="B107" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C107" s="149" t="s">
+      <c r="C107" s="155" t="s">
         <v>628</v>
       </c>
       <c r="D107" s="54" t="s">
@@ -7141,7 +7144,7 @@
       <c r="B108" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C108" s="148"/>
+      <c r="C108" s="154"/>
       <c r="D108" s="10" t="s">
         <v>284</v>
       </c>
@@ -7154,7 +7157,7 @@
       <c r="B109" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C109" s="149" t="s">
+      <c r="C109" s="155" t="s">
         <v>629</v>
       </c>
       <c r="D109" s="54" t="s">
@@ -7169,7 +7172,7 @@
       <c r="B110" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C110" s="148"/>
+      <c r="C110" s="154"/>
       <c r="D110" s="10" t="s">
         <v>373</v>
       </c>
@@ -7182,7 +7185,7 @@
       <c r="B111" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C111" s="149" t="s">
+      <c r="C111" s="155" t="s">
         <v>630</v>
       </c>
       <c r="D111" s="54" t="s">
@@ -7197,7 +7200,7 @@
       <c r="B112" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C112" s="148"/>
+      <c r="C112" s="154"/>
       <c r="D112" s="10" t="s">
         <v>341</v>
       </c>
@@ -7210,7 +7213,7 @@
       <c r="B113" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C113" s="149" t="s">
+      <c r="C113" s="155" t="s">
         <v>631</v>
       </c>
       <c r="D113" s="10" t="s">
@@ -7225,7 +7228,7 @@
       <c r="B114" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C114" s="148"/>
+      <c r="C114" s="154"/>
       <c r="D114" s="10" t="s">
         <v>374</v>
       </c>
@@ -7238,7 +7241,7 @@
       <c r="B115" s="7" t="s">
         <v>640</v>
       </c>
-      <c r="C115" s="147" t="s">
+      <c r="C115" s="153" t="s">
         <v>632</v>
       </c>
       <c r="D115" s="54" t="s">
@@ -7253,7 +7256,7 @@
       <c r="B116" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="C116" s="148"/>
+      <c r="C116" s="154"/>
       <c r="D116" s="10" t="s">
         <v>438</v>
       </c>
@@ -7266,7 +7269,7 @@
       <c r="B117" s="7" t="s">
         <v>688</v>
       </c>
-      <c r="C117" s="149" t="s">
+      <c r="C117" s="155" t="s">
         <v>633</v>
       </c>
       <c r="D117" s="54" t="s">
@@ -7281,7 +7284,7 @@
       <c r="B118" s="41" t="s">
         <v>689</v>
       </c>
-      <c r="C118" s="148"/>
+      <c r="C118" s="154"/>
       <c r="D118" s="10" t="s">
         <v>337</v>
       </c>
@@ -7294,7 +7297,7 @@
       <c r="B119" s="12" t="s">
         <v>690</v>
       </c>
-      <c r="C119" s="149" t="s">
+      <c r="C119" s="155" t="s">
         <v>634</v>
       </c>
       <c r="D119" s="54" t="s">
@@ -7309,7 +7312,7 @@
       <c r="B120" s="9" t="s">
         <v>691</v>
       </c>
-      <c r="C120" s="148"/>
+      <c r="C120" s="154"/>
       <c r="D120" s="10" t="s">
         <v>445</v>
       </c>
@@ -7322,7 +7325,7 @@
       <c r="B121" s="7" t="s">
         <v>692</v>
       </c>
-      <c r="C121" s="149" t="s">
+      <c r="C121" s="155" t="s">
         <v>635</v>
       </c>
       <c r="D121" s="54" t="s">
@@ -7337,7 +7340,7 @@
       <c r="B122" s="9" t="s">
         <v>693</v>
       </c>
-      <c r="C122" s="148"/>
+      <c r="C122" s="154"/>
       <c r="D122" s="10" t="s">
         <v>295</v>
       </c>
@@ -7348,6 +7351,10 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="C121:C122"/>
+    <mergeCell ref="C3:G3"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="C45:G45"/>
     <mergeCell ref="C107:C108"/>
@@ -7361,10 +7368,6 @@
     <mergeCell ref="C105:C106"/>
     <mergeCell ref="C111:C112"/>
     <mergeCell ref="C113:C114"/>
-    <mergeCell ref="C117:C118"/>
-    <mergeCell ref="C119:C120"/>
-    <mergeCell ref="C121:C122"/>
-    <mergeCell ref="C3:G3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -7489,7 +7492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F4207A-FD9A-4441-8D18-CA12DEE5B8C9}">
   <dimension ref="A2:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="D10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -7508,11 +7511,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="128" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -7581,11 +7584,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="B9" s="123" t="s">
+      <c r="B9" s="128" t="s">
         <v>211</v>
       </c>
-      <c r="C9" s="123"/>
-      <c r="D9" s="123"/>
+      <c r="C9" s="128"/>
+      <c r="D9" s="128"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -7761,11 +7764,11 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B18" s="123" t="s">
+      <c r="B18" s="128" t="s">
         <v>253</v>
       </c>
-      <c r="C18" s="123"/>
-      <c r="D18" s="123"/>
+      <c r="C18" s="128"/>
+      <c r="D18" s="128"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -7894,12 +7897,12 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B26" s="127" t="s">
+      <c r="B26" s="132" t="s">
         <v>484</v>
       </c>
-      <c r="C26" s="128"/>
-      <c r="D26" s="128"/>
-      <c r="E26" s="129"/>
+      <c r="C26" s="133"/>
+      <c r="D26" s="133"/>
+      <c r="E26" s="134"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
@@ -7931,7 +7934,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="130" t="s">
+      <c r="B29" s="135" t="s">
         <v>480</v>
       </c>
       <c r="C29" s="7">
@@ -7955,7 +7958,7 @@
       <c r="A30">
         <v>42</v>
       </c>
-      <c r="B30" s="131"/>
+      <c r="B30" s="136"/>
       <c r="C30" s="40">
         <v>2</v>
       </c>
@@ -7974,7 +7977,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="131"/>
+      <c r="B31" s="136"/>
       <c r="C31" s="40">
         <v>3</v>
       </c>
@@ -7993,7 +7996,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="132"/>
+      <c r="B32" s="137"/>
       <c r="C32" s="9">
         <v>4</v>
       </c>
@@ -8012,7 +8015,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="124" t="s">
+      <c r="B33" s="129" t="s">
         <v>481</v>
       </c>
       <c r="C33" s="12">
@@ -8036,7 +8039,7 @@
       <c r="A34">
         <v>46</v>
       </c>
-      <c r="B34" s="125"/>
+      <c r="B34" s="130"/>
       <c r="C34" s="40">
         <v>2</v>
       </c>
@@ -8055,7 +8058,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="126"/>
+      <c r="B35" s="131"/>
       <c r="C35" s="9">
         <v>3</v>
       </c>
@@ -8077,7 +8080,7 @@
       <c r="A36">
         <v>48</v>
       </c>
-      <c r="B36" s="133" t="s">
+      <c r="B36" s="138" t="s">
         <v>485</v>
       </c>
       <c r="C36" s="7">
@@ -8098,7 +8101,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="125"/>
+      <c r="B37" s="130"/>
       <c r="C37" s="40">
         <v>2</v>
       </c>
@@ -8117,7 +8120,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="126"/>
+      <c r="B38" s="131"/>
       <c r="C38" s="9">
         <v>3</v>
       </c>
@@ -8136,7 +8139,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="124" t="s">
+      <c r="B39" s="129" t="s">
         <v>481</v>
       </c>
       <c r="C39" s="12">
@@ -8156,7 +8159,7 @@
       <c r="A40">
         <v>52</v>
       </c>
-      <c r="B40" s="125"/>
+      <c r="B40" s="130"/>
       <c r="C40" s="55">
         <v>2</v>
       </c>
@@ -8171,7 +8174,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="126"/>
+      <c r="B41" s="131"/>
       <c r="C41" s="9">
         <v>3</v>
       </c>
@@ -8244,13 +8247,13 @@
   <sheetData>
     <row r="3" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
-      <c r="C3" s="123" t="s">
+      <c r="C3" s="128" t="s">
         <v>588</v>
       </c>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
     </row>
     <row r="4" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
@@ -8267,12 +8270,12 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="121" t="s">
+      <c r="H5" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="121"/>
-      <c r="J5" s="121"/>
-      <c r="K5" s="121"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="126"/>
+      <c r="K5" s="126"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="s">
@@ -9525,13 +9528,13 @@
     </row>
     <row r="39" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
-      <c r="C39" s="123" t="s">
+      <c r="C39" s="128" t="s">
         <v>625</v>
       </c>
-      <c r="D39" s="123"/>
-      <c r="E39" s="123"/>
-      <c r="F39" s="123"/>
-      <c r="G39" s="123"/>
+      <c r="D39" s="128"/>
+      <c r="E39" s="128"/>
+      <c r="F39" s="128"/>
+      <c r="G39" s="128"/>
     </row>
     <row r="40" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
@@ -10171,13 +10174,13 @@
     </row>
     <row r="68" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B68" s="3"/>
-      <c r="C68" s="123" t="s">
+      <c r="C68" s="128" t="s">
         <v>664</v>
       </c>
-      <c r="D68" s="123"/>
-      <c r="E68" s="123"/>
-      <c r="F68" s="123"/>
-      <c r="G68" s="123"/>
+      <c r="D68" s="128"/>
+      <c r="E68" s="128"/>
+      <c r="F68" s="128"/>
+      <c r="G68" s="128"/>
     </row>
     <row r="69" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B69" s="3"/>
@@ -10231,7 +10234,7 @@
       <c r="F72">
         <v>44</v>
       </c>
-      <c r="G72" s="155">
+      <c r="G72" s="122">
         <v>44197</v>
       </c>
       <c r="H72" t="str">
@@ -10255,7 +10258,7 @@
       <c r="F73">
         <v>44</v>
       </c>
-      <c r="G73" s="155">
+      <c r="G73" s="122">
         <v>44198</v>
       </c>
       <c r="H73" t="str">
@@ -10279,7 +10282,7 @@
       <c r="F74">
         <v>44</v>
       </c>
-      <c r="G74" s="155">
+      <c r="G74" s="122">
         <v>44199</v>
       </c>
       <c r="H74" t="str">
@@ -10303,7 +10306,7 @@
       <c r="F75">
         <v>44</v>
       </c>
-      <c r="G75" s="155">
+      <c r="G75" s="122">
         <v>44200</v>
       </c>
       <c r="H75" t="str">
@@ -10327,7 +10330,7 @@
       <c r="F76">
         <v>43</v>
       </c>
-      <c r="G76" s="155">
+      <c r="G76" s="122">
         <v>44201</v>
       </c>
       <c r="H76" t="str">
@@ -10351,7 +10354,7 @@
       <c r="F77">
         <v>43</v>
       </c>
-      <c r="G77" s="155">
+      <c r="G77" s="122">
         <v>44202</v>
       </c>
       <c r="H77" t="str">
@@ -10375,7 +10378,7 @@
       <c r="F78">
         <v>42</v>
       </c>
-      <c r="G78" s="155">
+      <c r="G78" s="122">
         <v>44203</v>
       </c>
       <c r="H78" t="str">
@@ -10399,7 +10402,7 @@
       <c r="F79">
         <v>42</v>
       </c>
-      <c r="G79" s="155">
+      <c r="G79" s="122">
         <v>44204</v>
       </c>
       <c r="H79" t="str">
@@ -10423,7 +10426,7 @@
       <c r="F80">
         <v>41</v>
       </c>
-      <c r="G80" s="155">
+      <c r="G80" s="122">
         <v>44205</v>
       </c>
       <c r="H80" t="str">
@@ -10447,7 +10450,7 @@
       <c r="F81">
         <v>41</v>
       </c>
-      <c r="G81" s="155">
+      <c r="G81" s="122">
         <v>44206</v>
       </c>
       <c r="H81" t="str">
@@ -10471,7 +10474,7 @@
       <c r="F82">
         <v>48</v>
       </c>
-      <c r="G82" s="155">
+      <c r="G82" s="122">
         <v>44207</v>
       </c>
       <c r="H82" t="str">
@@ -10495,7 +10498,7 @@
       <c r="F83">
         <v>48</v>
       </c>
-      <c r="G83" s="155">
+      <c r="G83" s="122">
         <v>44208</v>
       </c>
       <c r="H83" t="str">
@@ -10519,7 +10522,7 @@
       <c r="F84">
         <v>48</v>
       </c>
-      <c r="G84" s="155">
+      <c r="G84" s="122">
         <v>44209</v>
       </c>
       <c r="H84" t="str">
@@ -10543,7 +10546,7 @@
       <c r="F85">
         <v>48</v>
       </c>
-      <c r="G85" s="155">
+      <c r="G85" s="122">
         <v>44210</v>
       </c>
       <c r="H85" t="str">
@@ -10567,7 +10570,7 @@
       <c r="F86">
         <v>49</v>
       </c>
-      <c r="G86" s="155">
+      <c r="G86" s="122">
         <v>44211</v>
       </c>
       <c r="H86" t="str">
@@ -10591,7 +10594,7 @@
       <c r="F87">
         <v>49</v>
       </c>
-      <c r="G87" s="155">
+      <c r="G87" s="122">
         <v>44212</v>
       </c>
       <c r="H87" t="str">
@@ -10615,7 +10618,7 @@
       <c r="F88">
         <v>49</v>
       </c>
-      <c r="G88" s="155">
+      <c r="G88" s="122">
         <v>44213</v>
       </c>
       <c r="H88" t="str">
@@ -10639,7 +10642,7 @@
       <c r="F89">
         <v>49</v>
       </c>
-      <c r="G89" s="155">
+      <c r="G89" s="122">
         <v>44214</v>
       </c>
       <c r="H89" t="str">
@@ -10663,7 +10666,7 @@
       <c r="F90">
         <v>49</v>
       </c>
-      <c r="G90" s="155">
+      <c r="G90" s="122">
         <v>44215</v>
       </c>
       <c r="H90" t="str">
@@ -10687,7 +10690,7 @@
       <c r="F91">
         <v>49</v>
       </c>
-      <c r="G91" s="155">
+      <c r="G91" s="122">
         <v>44216</v>
       </c>
       <c r="H91" t="str">
@@ -10696,7 +10699,7 @@
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B92" s="134">
+      <c r="B92" s="139">
         <v>21</v>
       </c>
       <c r="C92" s="120" t="s">
@@ -10711,7 +10714,7 @@
       <c r="F92">
         <v>45</v>
       </c>
-      <c r="G92" s="155">
+      <c r="G92" s="122">
         <v>44217</v>
       </c>
       <c r="H92" t="str">
@@ -10720,7 +10723,7 @@
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B93" s="135"/>
+      <c r="B93" s="140"/>
       <c r="C93" s="120" t="s">
         <v>752</v>
       </c>
@@ -10733,7 +10736,7 @@
       <c r="F93">
         <v>53</v>
       </c>
-      <c r="G93" s="155">
+      <c r="G93" s="122">
         <v>44217</v>
       </c>
       <c r="H93" t="str">
@@ -10742,7 +10745,7 @@
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="134">
+      <c r="B94" s="139">
         <v>22</v>
       </c>
       <c r="C94" s="120" t="s">
@@ -10757,7 +10760,7 @@
       <c r="F94">
         <v>45</v>
       </c>
-      <c r="G94" s="155">
+      <c r="G94" s="122">
         <v>44219</v>
       </c>
       <c r="H94" t="str">
@@ -10766,7 +10769,7 @@
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="135"/>
+      <c r="B95" s="140"/>
       <c r="C95" s="120" t="s">
         <v>753</v>
       </c>
@@ -10779,7 +10782,7 @@
       <c r="F95">
         <v>53</v>
       </c>
-      <c r="G95" s="155">
+      <c r="G95" s="122">
         <v>44219</v>
       </c>
       <c r="H95" t="str">
@@ -10788,7 +10791,7 @@
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B96" s="134">
+      <c r="B96" s="139">
         <v>23</v>
       </c>
       <c r="C96" s="120" t="s">
@@ -10803,7 +10806,7 @@
       <c r="F96">
         <v>45</v>
       </c>
-      <c r="G96" s="155">
+      <c r="G96" s="122">
         <v>44221</v>
       </c>
       <c r="H96" t="str">
@@ -10812,7 +10815,7 @@
       </c>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B97" s="135"/>
+      <c r="B97" s="140"/>
       <c r="C97" s="120" t="s">
         <v>754</v>
       </c>
@@ -10825,7 +10828,7 @@
       <c r="F97">
         <v>53</v>
       </c>
-      <c r="G97" s="155">
+      <c r="G97" s="122">
         <v>44221</v>
       </c>
       <c r="H97" t="str">
@@ -10834,7 +10837,7 @@
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B98" s="134">
+      <c r="B98" s="139">
         <v>24</v>
       </c>
       <c r="C98" s="120" t="s">
@@ -10849,7 +10852,7 @@
       <c r="F98">
         <v>46</v>
       </c>
-      <c r="G98" s="155">
+      <c r="G98" s="122">
         <v>44223</v>
       </c>
       <c r="H98" t="str">
@@ -10858,7 +10861,7 @@
       </c>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B99" s="135"/>
+      <c r="B99" s="140"/>
       <c r="C99" s="120" t="s">
         <v>755</v>
       </c>
@@ -10871,7 +10874,7 @@
       <c r="F99">
         <v>52</v>
       </c>
-      <c r="G99" s="155">
+      <c r="G99" s="122">
         <v>44223</v>
       </c>
       <c r="H99" t="str">
@@ -10880,7 +10883,7 @@
       </c>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B100" s="134">
+      <c r="B100" s="139">
         <v>25</v>
       </c>
       <c r="C100" s="120" t="s">
@@ -10895,7 +10898,7 @@
       <c r="F100">
         <v>46</v>
       </c>
-      <c r="G100" s="155">
+      <c r="G100" s="122">
         <v>44225</v>
       </c>
       <c r="H100" t="str">
@@ -10904,7 +10907,7 @@
       </c>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B101" s="135"/>
+      <c r="B101" s="140"/>
       <c r="C101" s="120" t="s">
         <v>756</v>
       </c>
@@ -10917,7 +10920,7 @@
       <c r="F101">
         <v>52</v>
       </c>
-      <c r="G101" s="155">
+      <c r="G101" s="122">
         <v>44225</v>
       </c>
       <c r="H101" t="str">
@@ -10926,7 +10929,7 @@
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B102" s="134">
+      <c r="B102" s="139">
         <v>26</v>
       </c>
       <c r="C102" s="120" t="s">
@@ -10941,7 +10944,7 @@
       <c r="F102">
         <v>46</v>
       </c>
-      <c r="G102" s="155">
+      <c r="G102" s="122">
         <v>44227</v>
       </c>
       <c r="H102" t="str">
@@ -10950,7 +10953,7 @@
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B103" s="135"/>
+      <c r="B103" s="140"/>
       <c r="C103" s="120" t="s">
         <v>757</v>
       </c>
@@ -10963,7 +10966,7 @@
       <c r="F103">
         <v>52</v>
       </c>
-      <c r="G103" s="155">
+      <c r="G103" s="122">
         <v>44227</v>
       </c>
       <c r="H103" t="str">
@@ -10972,7 +10975,7 @@
       </c>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B104" s="134">
+      <c r="B104" s="139">
         <v>27</v>
       </c>
       <c r="C104" s="120" t="s">
@@ -10987,7 +10990,7 @@
       <c r="F104">
         <v>46</v>
       </c>
-      <c r="G104" s="155">
+      <c r="G104" s="122">
         <v>44229</v>
       </c>
       <c r="H104" t="str">
@@ -10996,7 +10999,7 @@
       </c>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B105" s="135"/>
+      <c r="B105" s="140"/>
       <c r="C105" s="120" t="s">
         <v>758</v>
       </c>
@@ -11009,7 +11012,7 @@
       <c r="F105">
         <v>51</v>
       </c>
-      <c r="G105" s="155">
+      <c r="G105" s="122">
         <v>44229</v>
       </c>
       <c r="H105" t="str">
@@ -11018,7 +11021,7 @@
       </c>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B106" s="134">
+      <c r="B106" s="139">
         <v>28</v>
       </c>
       <c r="C106" s="120" t="s">
@@ -11033,7 +11036,7 @@
       <c r="F106">
         <v>47</v>
       </c>
-      <c r="G106" s="155">
+      <c r="G106" s="122">
         <v>44231</v>
       </c>
       <c r="H106" t="str">
@@ -11042,7 +11045,7 @@
       </c>
     </row>
     <row r="107" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B107" s="135"/>
+      <c r="B107" s="140"/>
       <c r="C107" s="120" t="s">
         <v>759</v>
       </c>
@@ -11055,7 +11058,7 @@
       <c r="F107">
         <v>51</v>
       </c>
-      <c r="G107" s="155">
+      <c r="G107" s="122">
         <v>44231</v>
       </c>
       <c r="H107" t="str">
@@ -11064,7 +11067,7 @@
       </c>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B108" s="134">
+      <c r="B108" s="139">
         <v>29</v>
       </c>
       <c r="C108" s="120" t="s">
@@ -11079,7 +11082,7 @@
       <c r="F108">
         <v>47</v>
       </c>
-      <c r="G108" s="155">
+      <c r="G108" s="122">
         <v>44233</v>
       </c>
       <c r="H108" t="str">
@@ -11088,7 +11091,7 @@
       </c>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B109" s="135"/>
+      <c r="B109" s="140"/>
       <c r="C109" s="120" t="s">
         <v>632</v>
       </c>
@@ -11101,7 +11104,7 @@
       <c r="F109">
         <v>51</v>
       </c>
-      <c r="G109" s="155">
+      <c r="G109" s="122">
         <v>44233</v>
       </c>
       <c r="H109" t="str">
@@ -11110,7 +11113,7 @@
       </c>
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B110" s="134">
+      <c r="B110" s="139">
         <v>30</v>
       </c>
       <c r="C110" s="120" t="s">
@@ -11125,7 +11128,7 @@
       <c r="F110">
         <v>47</v>
       </c>
-      <c r="G110" s="155">
+      <c r="G110" s="122">
         <v>44235</v>
       </c>
       <c r="H110" t="str">
@@ -11134,7 +11137,7 @@
       </c>
     </row>
     <row r="111" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B111" s="135"/>
+      <c r="B111" s="140"/>
       <c r="C111" s="120" t="s">
         <v>634</v>
       </c>
@@ -11147,7 +11150,7 @@
       <c r="F111">
         <v>53</v>
       </c>
-      <c r="G111" s="155">
+      <c r="G111" s="122">
         <v>44235</v>
       </c>
       <c r="H111" t="str">
@@ -11158,6 +11161,11 @@
   </sheetData>
   <autoFilter ref="B71:F111" xr:uid="{DE5F5F80-836B-41FC-A793-6D21B74ED654}"/>
   <mergeCells count="14">
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="C68:G68"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="C39:G39"/>
     <mergeCell ref="B110:B111"/>
     <mergeCell ref="B94:B95"/>
     <mergeCell ref="B96:B97"/>
@@ -11167,11 +11175,6 @@
     <mergeCell ref="B104:B105"/>
     <mergeCell ref="B106:B107"/>
     <mergeCell ref="B108:B109"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="C68:G68"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="C39:G39"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -11380,11 +11383,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="K2" s="123" t="s">
+      <c r="K2" s="128" t="s">
         <v>490</v>
       </c>
-      <c r="L2" s="123"/>
-      <c r="M2" s="123"/>
+      <c r="L2" s="128"/>
+      <c r="M2" s="128"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
@@ -11694,7 +11697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60A9011-4F7D-4949-BA51-785306AAE4EA}">
   <dimension ref="B2:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -11716,11 +11719,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="C2" s="123" t="s">
+      <c r="C2" s="128" t="s">
         <v>841</v>
       </c>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
     </row>
     <row r="3" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="C3" s="53"/>
@@ -11730,18 +11733,18 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="121" t="s">
+      <c r="E4" s="126" t="s">
         <v>842</v>
       </c>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121" t="s">
+      <c r="F4" s="126"/>
+      <c r="G4" s="126" t="s">
         <v>843</v>
       </c>
-      <c r="H4" s="121"/>
-      <c r="I4" s="121" t="s">
+      <c r="H4" s="126"/>
+      <c r="I4" s="126" t="s">
         <v>844</v>
       </c>
-      <c r="J4" s="121"/>
+      <c r="J4" s="126"/>
       <c r="K4" s="1"/>
       <c r="L4" s="108"/>
     </row>
@@ -11794,22 +11797,22 @@
       <c r="D6" s="13" t="s">
         <v>496</v>
       </c>
-      <c r="E6" s="156">
+      <c r="E6" s="123">
         <v>44237</v>
       </c>
-      <c r="F6" s="156">
+      <c r="F6" s="123">
         <v>44252</v>
       </c>
-      <c r="G6" s="156">
+      <c r="G6" s="123">
         <v>44238</v>
       </c>
-      <c r="H6" s="156">
+      <c r="H6" s="123">
         <v>44247</v>
       </c>
-      <c r="I6" s="156">
+      <c r="I6" s="123">
         <v>44248</v>
       </c>
-      <c r="J6" s="156">
+      <c r="J6" s="123">
         <v>44251</v>
       </c>
       <c r="K6" s="110" t="s">
@@ -11833,22 +11836,22 @@
       <c r="D7" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="E7" s="157">
+      <c r="E7" s="124">
         <v>44237</v>
       </c>
-      <c r="F7" s="157">
+      <c r="F7" s="124">
         <v>44252</v>
       </c>
-      <c r="G7" s="156">
+      <c r="G7" s="123">
         <v>44238</v>
       </c>
-      <c r="H7" s="156">
+      <c r="H7" s="123">
         <v>44247</v>
       </c>
-      <c r="I7" s="156">
+      <c r="I7" s="123">
         <v>44248</v>
       </c>
-      <c r="J7" s="156">
+      <c r="J7" s="123">
         <v>44251</v>
       </c>
       <c r="K7" s="111" t="s">
@@ -11872,22 +11875,22 @@
       <c r="D8" s="10" t="s">
         <v>507</v>
       </c>
-      <c r="E8" s="158">
+      <c r="E8" s="125">
         <v>44236</v>
       </c>
-      <c r="F8" s="158">
+      <c r="F8" s="125">
         <v>44253</v>
       </c>
-      <c r="G8" s="158">
+      <c r="G8" s="125">
         <v>44237</v>
       </c>
-      <c r="H8" s="158">
+      <c r="H8" s="125">
         <v>44246</v>
       </c>
-      <c r="I8" s="158">
+      <c r="I8" s="125">
         <v>44247</v>
       </c>
-      <c r="J8" s="158">
+      <c r="J8" s="125">
         <v>44250</v>
       </c>
       <c r="K8" s="112" t="s">
@@ -11911,22 +11914,22 @@
       <c r="D9" s="13" t="s">
         <v>514</v>
       </c>
-      <c r="E9" s="156">
+      <c r="E9" s="123">
         <v>44237</v>
       </c>
-      <c r="F9" s="156">
+      <c r="F9" s="123">
         <v>44252</v>
       </c>
-      <c r="G9" s="156">
+      <c r="G9" s="123">
         <v>44238</v>
       </c>
-      <c r="H9" s="156">
+      <c r="H9" s="123">
         <v>44247</v>
       </c>
-      <c r="I9" s="156">
+      <c r="I9" s="123">
         <v>44248</v>
       </c>
-      <c r="J9" s="156">
+      <c r="J9" s="123">
         <v>44251</v>
       </c>
       <c r="K9" s="114" t="s">
@@ -11950,22 +11953,22 @@
       <c r="D10" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="E10" s="158">
+      <c r="E10" s="125">
         <v>44236</v>
       </c>
-      <c r="F10" s="158">
+      <c r="F10" s="125">
         <v>44253</v>
       </c>
-      <c r="G10" s="158">
+      <c r="G10" s="125">
         <v>44237</v>
       </c>
-      <c r="H10" s="158">
+      <c r="H10" s="125">
         <v>44246</v>
       </c>
-      <c r="I10" s="158">
+      <c r="I10" s="125">
         <v>44247</v>
       </c>
-      <c r="J10" s="158">
+      <c r="J10" s="125">
         <v>44250</v>
       </c>
       <c r="K10" s="115" t="s">
@@ -11985,11 +11988,11 @@
       <c r="K11" s="100"/>
     </row>
     <row r="13" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="128" t="s">
         <v>830</v>
       </c>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
+      <c r="C13" s="128"/>
+      <c r="D13" s="128"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
@@ -12126,11 +12129,11 @@
       <c r="B4" s="116" t="s">
         <v>844</v>
       </c>
-      <c r="E4" s="136" t="s">
+      <c r="E4" s="141" t="s">
         <v>856</v>
       </c>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
+      <c r="F4" s="141"/>
+      <c r="G4" s="141"/>
       <c r="H4" s="53"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
@@ -13985,16 +13988,16 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="121" t="s">
+      <c r="H4" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="121"/>
-      <c r="J4" s="121"/>
-      <c r="K4" s="121"/>
-      <c r="L4" s="121" t="s">
+      <c r="I4" s="126"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="126"/>
+      <c r="L4" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="121"/>
+      <c r="M4" s="126"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -14264,11 +14267,11 @@
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F14" s="122" t="s">
+      <c r="F14" s="127" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="122"/>
-      <c r="H14" s="122"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="127"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -14300,7 +14303,7 @@
       <c r="B17" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="134">
+      <c r="C17" s="139">
         <v>111222333</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -14324,7 +14327,7 @@
       <c r="B18" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="137"/>
+      <c r="C18" s="142"/>
       <c r="D18" s="2" t="s">
         <v>105</v>
       </c>
@@ -14346,7 +14349,7 @@
       <c r="B19" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="137"/>
+      <c r="C19" s="142"/>
       <c r="D19" s="2" t="s">
         <v>106</v>
       </c>
@@ -14368,7 +14371,7 @@
       <c r="B20" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="137"/>
+      <c r="C20" s="142"/>
       <c r="D20" s="2" t="s">
         <v>107</v>
       </c>
@@ -14390,7 +14393,7 @@
       <c r="B21" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="137"/>
+      <c r="C21" s="142"/>
       <c r="D21" s="2" t="s">
         <v>108</v>
       </c>
@@ -14412,7 +14415,7 @@
       <c r="B22" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="138"/>
+      <c r="C22" s="143"/>
       <c r="D22" s="9" t="s">
         <v>109</v>
       </c>
@@ -14434,7 +14437,7 @@
       <c r="B23" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="137">
+      <c r="C23" s="142">
         <v>111222444</v>
       </c>
       <c r="D23" s="7" t="s">
@@ -14458,7 +14461,7 @@
       <c r="B24" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="137"/>
+      <c r="C24" s="142"/>
       <c r="D24" s="2" t="s">
         <v>134</v>
       </c>
@@ -14480,7 +14483,7 @@
       <c r="B25" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="137"/>
+      <c r="C25" s="142"/>
       <c r="D25" s="2" t="s">
         <v>135</v>
       </c>
@@ -14502,7 +14505,7 @@
       <c r="B26" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="137"/>
+      <c r="C26" s="142"/>
       <c r="D26" s="2" t="s">
         <v>136</v>
       </c>
@@ -14524,7 +14527,7 @@
       <c r="B27" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="137"/>
+      <c r="C27" s="142"/>
       <c r="D27" s="2" t="s">
         <v>137</v>
       </c>
@@ -14546,7 +14549,7 @@
       <c r="B28" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="138"/>
+      <c r="C28" s="143"/>
       <c r="D28" s="9" t="s">
         <v>138</v>
       </c>
@@ -14567,7 +14570,7 @@
       <c r="B29" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C29" s="139">
+      <c r="C29" s="144">
         <v>111222555</v>
       </c>
       <c r="D29" s="12" t="s">
@@ -14590,7 +14593,7 @@
       <c r="B30" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="137"/>
+      <c r="C30" s="142"/>
       <c r="D30" s="2" t="s">
         <v>139</v>
       </c>
@@ -14611,7 +14614,7 @@
       <c r="B31" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="137"/>
+      <c r="C31" s="142"/>
       <c r="D31" s="2" t="s">
         <v>140</v>
       </c>
@@ -14632,7 +14635,7 @@
       <c r="B32" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="137"/>
+      <c r="C32" s="142"/>
       <c r="D32" s="2" t="s">
         <v>141</v>
       </c>
@@ -14653,7 +14656,7 @@
       <c r="B33" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C33" s="137"/>
+      <c r="C33" s="142"/>
       <c r="D33" s="2" t="s">
         <v>142</v>
       </c>
@@ -14675,7 +14678,7 @@
       <c r="B34" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="138"/>
+      <c r="C34" s="143"/>
       <c r="D34" s="9" t="s">
         <v>143</v>
       </c>
@@ -14697,7 +14700,7 @@
       <c r="B35" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="137">
+      <c r="C35" s="142">
         <v>111222666</v>
       </c>
       <c r="D35" s="7" t="s">
@@ -14721,7 +14724,7 @@
       <c r="B36" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="137"/>
+      <c r="C36" s="142"/>
       <c r="D36" s="2" t="s">
         <v>144</v>
       </c>
@@ -14743,7 +14746,7 @@
       <c r="B37" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="137"/>
+      <c r="C37" s="142"/>
       <c r="D37" s="2" t="s">
         <v>145</v>
       </c>
@@ -14765,7 +14768,7 @@
       <c r="B38" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C38" s="137"/>
+      <c r="C38" s="142"/>
       <c r="D38" s="2" t="s">
         <v>146</v>
       </c>
@@ -14787,7 +14790,7 @@
       <c r="B39" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="C39" s="137"/>
+      <c r="C39" s="142"/>
       <c r="D39" s="2" t="s">
         <v>147</v>
       </c>
@@ -14809,7 +14812,7 @@
       <c r="B40" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="138"/>
+      <c r="C40" s="143"/>
       <c r="D40" s="9" t="s">
         <v>148</v>
       </c>
@@ -14831,7 +14834,7 @@
       <c r="B41" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="137">
+      <c r="C41" s="142">
         <v>111222777</v>
       </c>
       <c r="D41" s="7" t="s">
@@ -14855,7 +14858,7 @@
       <c r="B42" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="C42" s="137"/>
+      <c r="C42" s="142"/>
       <c r="D42" s="2" t="s">
         <v>149</v>
       </c>
@@ -14877,7 +14880,7 @@
       <c r="B43" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="137"/>
+      <c r="C43" s="142"/>
       <c r="D43" s="2" t="s">
         <v>150</v>
       </c>
@@ -14899,7 +14902,7 @@
       <c r="B44" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C44" s="137"/>
+      <c r="C44" s="142"/>
       <c r="D44" s="2" t="s">
         <v>151</v>
       </c>
@@ -14921,7 +14924,7 @@
       <c r="B45" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="C45" s="137"/>
+      <c r="C45" s="142"/>
       <c r="D45" s="2" t="s">
         <v>152</v>
       </c>
@@ -14942,7 +14945,7 @@
       <c r="B46" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C46" s="138"/>
+      <c r="C46" s="143"/>
       <c r="D46" s="9" t="s">
         <v>153</v>
       </c>
@@ -14963,7 +14966,7 @@
       <c r="B47" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="139">
+      <c r="C47" s="144">
         <v>111222888</v>
       </c>
       <c r="D47" s="12" t="s">
@@ -14986,7 +14989,7 @@
       <c r="B48" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="137"/>
+      <c r="C48" s="142"/>
       <c r="D48" s="2" t="s">
         <v>154</v>
       </c>
@@ -15007,7 +15010,7 @@
       <c r="B49" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="137"/>
+      <c r="C49" s="142"/>
       <c r="D49" s="2" t="s">
         <v>155</v>
       </c>
@@ -15028,7 +15031,7 @@
       <c r="B50" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="C50" s="137"/>
+      <c r="C50" s="142"/>
       <c r="D50" s="2" t="s">
         <v>156</v>
       </c>
@@ -15049,7 +15052,7 @@
       <c r="B51" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C51" s="137"/>
+      <c r="C51" s="142"/>
       <c r="D51" s="2" t="s">
         <v>157</v>
       </c>
@@ -15070,7 +15073,7 @@
       <c r="B52" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C52" s="138"/>
+      <c r="C52" s="143"/>
       <c r="D52" s="9" t="s">
         <v>158</v>
       </c>
@@ -15165,8 +15168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7606E586-509B-4141-B06E-3D5BBAD72C5F}">
   <dimension ref="A2:L90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="F16" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15184,11 +15187,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="128" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -15275,11 +15278,11 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="B12" s="123" t="s">
+      <c r="B12" s="128" t="s">
         <v>211</v>
       </c>
-      <c r="C12" s="123"/>
-      <c r="D12" s="123"/>
+      <c r="C12" s="128"/>
+      <c r="D12" s="128"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15308,19 +15311,19 @@
       <c r="G14" s="40" t="s">
         <v>697</v>
       </c>
-      <c r="I14" s="123" t="s">
+      <c r="I14" s="128" t="s">
         <v>484</v>
       </c>
-      <c r="J14" s="123"/>
-      <c r="K14" s="123"/>
-      <c r="L14" s="123"/>
+      <c r="J14" s="128"/>
+      <c r="K14" s="128"/>
+      <c r="L14" s="128"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
       <c r="B15" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="146" t="s">
+      <c r="C15" s="152" t="s">
         <v>204</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -15346,7 +15349,7 @@
       <c r="B16" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="147"/>
+      <c r="C16" s="153"/>
       <c r="D16" s="2" t="s">
         <v>236</v>
       </c>
@@ -15378,7 +15381,7 @@
       <c r="B17" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="148"/>
+      <c r="C17" s="154"/>
       <c r="D17" s="9" t="s">
         <v>237</v>
       </c>
@@ -15391,7 +15394,7 @@
       <c r="G17" s="40">
         <v>3</v>
       </c>
-      <c r="I17" s="125" t="s">
+      <c r="I17" s="130" t="s">
         <v>480</v>
       </c>
       <c r="J17" s="25">
@@ -15409,7 +15412,7 @@
       <c r="B18" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="147" t="s">
+      <c r="C18" s="153" t="s">
         <v>205</v>
       </c>
       <c r="D18" s="7" t="s">
@@ -15425,7 +15428,7 @@
       <c r="G18" s="40">
         <v>1</v>
       </c>
-      <c r="I18" s="125"/>
+      <c r="I18" s="130"/>
       <c r="J18" s="25">
         <v>2</v>
       </c>
@@ -15441,7 +15444,7 @@
       <c r="B19" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="147"/>
+      <c r="C19" s="153"/>
       <c r="D19" s="2" t="s">
         <v>239</v>
       </c>
@@ -15455,7 +15458,7 @@
       <c r="G19" s="40">
         <v>2</v>
       </c>
-      <c r="I19" s="126"/>
+      <c r="I19" s="131"/>
       <c r="J19" s="9">
         <v>3</v>
       </c>
@@ -15471,7 +15474,7 @@
       <c r="B20" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="148"/>
+      <c r="C20" s="154"/>
       <c r="D20" s="9" t="s">
         <v>240</v>
       </c>
@@ -15485,7 +15488,7 @@
       <c r="G20" s="40">
         <v>3</v>
       </c>
-      <c r="I20" s="124" t="s">
+      <c r="I20" s="129" t="s">
         <v>481</v>
       </c>
       <c r="J20" s="7">
@@ -15503,7 +15506,7 @@
       <c r="B21" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="147" t="s">
+      <c r="C21" s="153" t="s">
         <v>206</v>
       </c>
       <c r="D21" s="7" t="s">
@@ -15518,7 +15521,7 @@
       <c r="G21" s="40">
         <v>2</v>
       </c>
-      <c r="I21" s="125"/>
+      <c r="I21" s="130"/>
       <c r="J21" s="25">
         <v>2</v>
       </c>
@@ -15534,7 +15537,7 @@
       <c r="B22" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="147"/>
+      <c r="C22" s="153"/>
       <c r="D22" s="2" t="s">
         <v>242</v>
       </c>
@@ -15547,7 +15550,7 @@
       <c r="G22" s="40">
         <v>2</v>
       </c>
-      <c r="I22" s="125"/>
+      <c r="I22" s="130"/>
       <c r="J22" s="25">
         <v>3</v>
       </c>
@@ -15563,7 +15566,7 @@
       <c r="B23" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="147"/>
+      <c r="C23" s="153"/>
       <c r="D23" s="9" t="s">
         <v>243</v>
       </c>
@@ -15576,7 +15579,7 @@
       <c r="G23" s="40">
         <v>2</v>
       </c>
-      <c r="I23" s="126"/>
+      <c r="I23" s="131"/>
       <c r="J23" s="9">
         <v>4</v>
       </c>
@@ -15592,7 +15595,7 @@
       <c r="B24" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="149" t="s">
+      <c r="C24" s="155" t="s">
         <v>207</v>
       </c>
       <c r="D24" s="7" t="s">
@@ -15607,7 +15610,7 @@
       <c r="G24" s="40">
         <v>2</v>
       </c>
-      <c r="I24" s="124" t="s">
+      <c r="I24" s="129" t="s">
         <v>485</v>
       </c>
       <c r="J24" s="7">
@@ -15625,7 +15628,7 @@
       <c r="B25" s="86" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="147"/>
+      <c r="C25" s="153"/>
       <c r="D25" s="2" t="s">
         <v>245</v>
       </c>
@@ -15638,7 +15641,7 @@
       <c r="G25" s="40">
         <v>2</v>
       </c>
-      <c r="I25" s="125"/>
+      <c r="I25" s="130"/>
       <c r="J25" s="25">
         <v>2</v>
       </c>
@@ -15654,7 +15657,7 @@
       <c r="B26" s="87" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="148"/>
+      <c r="C26" s="154"/>
       <c r="D26" s="9" t="s">
         <v>246</v>
       </c>
@@ -15667,7 +15670,7 @@
       <c r="G26" s="40">
         <v>2</v>
       </c>
-      <c r="I26" s="125"/>
+      <c r="I26" s="130"/>
       <c r="J26" s="25">
         <v>3</v>
       </c>
@@ -15683,7 +15686,7 @@
       <c r="B27" s="88" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="147" t="s">
+      <c r="C27" s="153" t="s">
         <v>208</v>
       </c>
       <c r="D27" s="7" t="s">
@@ -15698,7 +15701,7 @@
       <c r="G27" s="40">
         <v>1</v>
       </c>
-      <c r="I27" s="126"/>
+      <c r="I27" s="131"/>
       <c r="J27" s="9">
         <v>4</v>
       </c>
@@ -15714,7 +15717,7 @@
       <c r="B28" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="147"/>
+      <c r="C28" s="153"/>
       <c r="D28" s="2" t="s">
         <v>248</v>
       </c>
@@ -15727,7 +15730,7 @@
       <c r="G28" s="40">
         <v>1</v>
       </c>
-      <c r="I28" s="124" t="s">
+      <c r="I28" s="129" t="s">
         <v>486</v>
       </c>
       <c r="J28" s="12">
@@ -15745,7 +15748,7 @@
       <c r="B29" s="89" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="147"/>
+      <c r="C29" s="153"/>
       <c r="D29" s="9" t="s">
         <v>249</v>
       </c>
@@ -15758,7 +15761,7 @@
       <c r="G29" s="40">
         <v>1</v>
       </c>
-      <c r="I29" s="125"/>
+      <c r="I29" s="130"/>
       <c r="J29" s="25">
         <v>2</v>
       </c>
@@ -15774,7 +15777,7 @@
       <c r="B30" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="149" t="s">
+      <c r="C30" s="155" t="s">
         <v>209</v>
       </c>
       <c r="D30" s="7" t="s">
@@ -15789,7 +15792,7 @@
       <c r="G30" s="40">
         <v>2</v>
       </c>
-      <c r="I30" s="126"/>
+      <c r="I30" s="131"/>
       <c r="J30" s="9">
         <v>3</v>
       </c>
@@ -15805,7 +15808,7 @@
       <c r="B31" s="86" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="147" t="s">
+      <c r="C31" s="153" t="s">
         <v>215</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -15820,7 +15823,7 @@
       <c r="G31" s="40">
         <v>2</v>
       </c>
-      <c r="I31" s="133" t="s">
+      <c r="I31" s="138" t="s">
         <v>487</v>
       </c>
       <c r="J31" s="7">
@@ -15837,7 +15840,7 @@
       <c r="B32" s="90" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="148" t="s">
+      <c r="C32" s="154" t="s">
         <v>216</v>
       </c>
       <c r="D32" s="9" t="s">
@@ -15852,7 +15855,7 @@
       <c r="G32" s="40">
         <v>1</v>
       </c>
-      <c r="I32" s="125"/>
+      <c r="I32" s="130"/>
       <c r="J32" s="25">
         <v>2</v>
       </c>
@@ -15864,7 +15867,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I33" s="126"/>
+      <c r="I33" s="131"/>
       <c r="J33" s="9">
         <v>3</v>
       </c>
@@ -15876,11 +15879,11 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="B34" s="123" t="s">
+      <c r="B34" s="128" t="s">
         <v>253</v>
       </c>
-      <c r="C34" s="123"/>
-      <c r="D34" s="123"/>
+      <c r="C34" s="128"/>
+      <c r="D34" s="128"/>
       <c r="E34" s="3"/>
     </row>
     <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15915,7 +15918,7 @@
       <c r="B37" s="35" t="s">
         <v>255</v>
       </c>
-      <c r="C37" s="143" t="s">
+      <c r="C37" s="147" t="s">
         <v>235</v>
       </c>
       <c r="D37" s="33" t="s">
@@ -15927,7 +15930,7 @@
       <c r="F37" s="30" t="s">
         <v>258</v>
       </c>
-      <c r="G37" s="140" t="s">
+      <c r="G37" s="156" t="s">
         <v>485</v>
       </c>
     </row>
@@ -15936,7 +15939,7 @@
       <c r="B38" s="35" t="s">
         <v>273</v>
       </c>
-      <c r="C38" s="144"/>
+      <c r="C38" s="145"/>
       <c r="D38" s="31" t="s">
         <v>264</v>
       </c>
@@ -15946,14 +15949,14 @@
       <c r="F38" s="31" t="s">
         <v>259</v>
       </c>
-      <c r="G38" s="141"/>
+      <c r="G38" s="157"/>
     </row>
     <row r="39" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="23"/>
       <c r="B39" s="36" t="s">
         <v>274</v>
       </c>
-      <c r="C39" s="145"/>
+      <c r="C39" s="146"/>
       <c r="D39" s="32" t="s">
         <v>265</v>
       </c>
@@ -15963,14 +15966,14 @@
       <c r="F39" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="G39" s="142"/>
+      <c r="G39" s="158"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
       <c r="B40" s="35" t="s">
         <v>277</v>
       </c>
-      <c r="C40" s="144" t="s">
+      <c r="C40" s="145" t="s">
         <v>236</v>
       </c>
       <c r="D40" s="30" t="s">
@@ -15982,7 +15985,7 @@
       <c r="F40" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="G40" s="140" t="s">
+      <c r="G40" s="156" t="s">
         <v>485</v>
       </c>
     </row>
@@ -15991,7 +15994,7 @@
       <c r="B41" s="35" t="s">
         <v>278</v>
       </c>
-      <c r="C41" s="144"/>
+      <c r="C41" s="145"/>
       <c r="D41" s="31" t="s">
         <v>275</v>
       </c>
@@ -16001,14 +16004,14 @@
       <c r="F41" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="G41" s="141"/>
+      <c r="G41" s="157"/>
     </row>
     <row r="42" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="23"/>
       <c r="B42" s="36" t="s">
         <v>279</v>
       </c>
-      <c r="C42" s="145"/>
+      <c r="C42" s="146"/>
       <c r="D42" s="32" t="s">
         <v>276</v>
       </c>
@@ -16018,14 +16021,14 @@
       <c r="F42" s="32" t="s">
         <v>272</v>
       </c>
-      <c r="G42" s="142"/>
+      <c r="G42" s="158"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="23"/>
       <c r="B43" s="35" t="s">
         <v>280</v>
       </c>
-      <c r="C43" s="144" t="s">
+      <c r="C43" s="145" t="s">
         <v>237</v>
       </c>
       <c r="D43" s="30" t="s">
@@ -16037,7 +16040,7 @@
       <c r="F43" s="30" t="s">
         <v>287</v>
       </c>
-      <c r="G43" s="140" t="s">
+      <c r="G43" s="156" t="s">
         <v>485</v>
       </c>
     </row>
@@ -16046,7 +16049,7 @@
       <c r="B44" s="35" t="s">
         <v>281</v>
       </c>
-      <c r="C44" s="144"/>
+      <c r="C44" s="145"/>
       <c r="D44" s="31" t="s">
         <v>284</v>
       </c>
@@ -16056,14 +16059,14 @@
       <c r="F44" s="31" t="s">
         <v>289</v>
       </c>
-      <c r="G44" s="141"/>
+      <c r="G44" s="157"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="23"/>
       <c r="B45" s="36" t="s">
         <v>282</v>
       </c>
-      <c r="C45" s="145"/>
+      <c r="C45" s="146"/>
       <c r="D45" s="32" t="s">
         <v>285</v>
       </c>
@@ -16073,14 +16076,14 @@
       <c r="F45" s="32" t="s">
         <v>498</v>
       </c>
-      <c r="G45" s="142"/>
+      <c r="G45" s="158"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="23"/>
       <c r="B46" s="35" t="s">
         <v>300</v>
       </c>
-      <c r="C46" s="144" t="s">
+      <c r="C46" s="145" t="s">
         <v>238</v>
       </c>
       <c r="D46" s="30" t="s">
@@ -16092,7 +16095,7 @@
       <c r="F46" s="30" t="s">
         <v>312</v>
       </c>
-      <c r="G46" s="140" t="s">
+      <c r="G46" s="156" t="s">
         <v>480</v>
       </c>
     </row>
@@ -16101,7 +16104,7 @@
       <c r="B47" s="35" t="s">
         <v>301</v>
       </c>
-      <c r="C47" s="144"/>
+      <c r="C47" s="145"/>
       <c r="D47" s="31" t="s">
         <v>292</v>
       </c>
@@ -16111,14 +16114,14 @@
       <c r="F47" s="31" t="s">
         <v>313</v>
       </c>
-      <c r="G47" s="141"/>
+      <c r="G47" s="157"/>
     </row>
     <row r="48" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="23"/>
       <c r="B48" s="36" t="s">
         <v>302</v>
       </c>
-      <c r="C48" s="145"/>
+      <c r="C48" s="146"/>
       <c r="D48" s="32" t="s">
         <v>293</v>
       </c>
@@ -16128,14 +16131,14 @@
       <c r="F48" s="32" t="s">
         <v>314</v>
       </c>
-      <c r="G48" s="142"/>
+      <c r="G48" s="158"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="23"/>
       <c r="B49" s="35" t="s">
         <v>303</v>
       </c>
-      <c r="C49" s="144" t="s">
+      <c r="C49" s="145" t="s">
         <v>239</v>
       </c>
       <c r="D49" s="30" t="s">
@@ -16147,7 +16150,7 @@
       <c r="F49" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="G49" s="140" t="s">
+      <c r="G49" s="156" t="s">
         <v>480</v>
       </c>
     </row>
@@ -16156,7 +16159,7 @@
       <c r="B50" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="C50" s="144"/>
+      <c r="C50" s="145"/>
       <c r="D50" s="31" t="s">
         <v>295</v>
       </c>
@@ -16166,14 +16169,14 @@
       <c r="F50" s="31" t="s">
         <v>319</v>
       </c>
-      <c r="G50" s="141"/>
+      <c r="G50" s="157"/>
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="23"/>
       <c r="B51" s="36" t="s">
         <v>305</v>
       </c>
-      <c r="C51" s="145"/>
+      <c r="C51" s="146"/>
       <c r="D51" s="32" t="s">
         <v>296</v>
       </c>
@@ -16183,14 +16186,14 @@
       <c r="F51" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="G51" s="142"/>
+      <c r="G51" s="158"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="23"/>
       <c r="B52" s="35" t="s">
         <v>306</v>
       </c>
-      <c r="C52" s="143" t="s">
+      <c r="C52" s="147" t="s">
         <v>240</v>
       </c>
       <c r="D52" s="30" t="s">
@@ -16202,7 +16205,7 @@
       <c r="F52" s="30" t="s">
         <v>324</v>
       </c>
-      <c r="G52" s="140" t="s">
+      <c r="G52" s="156" t="s">
         <v>480</v>
       </c>
     </row>
@@ -16211,7 +16214,7 @@
       <c r="B53" s="35" t="s">
         <v>307</v>
       </c>
-      <c r="C53" s="144"/>
+      <c r="C53" s="145"/>
       <c r="D53" s="31" t="s">
         <v>298</v>
       </c>
@@ -16221,14 +16224,14 @@
       <c r="F53" s="31" t="s">
         <v>325</v>
       </c>
-      <c r="G53" s="141"/>
+      <c r="G53" s="157"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="23"/>
       <c r="B54" s="20" t="s">
         <v>308</v>
       </c>
-      <c r="C54" s="150"/>
+      <c r="C54" s="148"/>
       <c r="D54" s="32" t="s">
         <v>299</v>
       </c>
@@ -16238,13 +16241,13 @@
       <c r="F54" s="32" t="s">
         <v>326</v>
       </c>
-      <c r="G54" s="142"/>
+      <c r="G54" s="158"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B55" s="35" t="s">
         <v>327</v>
       </c>
-      <c r="C55" s="144" t="s">
+      <c r="C55" s="145" t="s">
         <v>241</v>
       </c>
       <c r="D55" s="30" t="s">
@@ -16256,7 +16259,7 @@
       <c r="F55" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="G55" s="140" t="s">
+      <c r="G55" s="156" t="s">
         <v>481</v>
       </c>
     </row>
@@ -16264,7 +16267,7 @@
       <c r="B56" s="35" t="s">
         <v>328</v>
       </c>
-      <c r="C56" s="144"/>
+      <c r="C56" s="145"/>
       <c r="D56" s="31" t="s">
         <v>337</v>
       </c>
@@ -16274,13 +16277,13 @@
       <c r="F56" s="31" t="s">
         <v>349</v>
       </c>
-      <c r="G56" s="141"/>
+      <c r="G56" s="157"/>
     </row>
     <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="36" t="s">
         <v>329</v>
       </c>
-      <c r="C57" s="145"/>
+      <c r="C57" s="146"/>
       <c r="D57" s="32" t="s">
         <v>338</v>
       </c>
@@ -16290,13 +16293,13 @@
       <c r="F57" s="32" t="s">
         <v>350</v>
       </c>
-      <c r="G57" s="142"/>
+      <c r="G57" s="158"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B58" s="35" t="s">
         <v>330</v>
       </c>
-      <c r="C58" s="144" t="s">
+      <c r="C58" s="145" t="s">
         <v>242</v>
       </c>
       <c r="D58" s="30" t="s">
@@ -16308,7 +16311,7 @@
       <c r="F58" s="30" t="s">
         <v>354</v>
       </c>
-      <c r="G58" s="140" t="s">
+      <c r="G58" s="156" t="s">
         <v>481</v>
       </c>
     </row>
@@ -16316,7 +16319,7 @@
       <c r="B59" s="35" t="s">
         <v>331</v>
       </c>
-      <c r="C59" s="144"/>
+      <c r="C59" s="145"/>
       <c r="D59" s="31" t="s">
         <v>340</v>
       </c>
@@ -16326,13 +16329,13 @@
       <c r="F59" s="31" t="s">
         <v>355</v>
       </c>
-      <c r="G59" s="141"/>
+      <c r="G59" s="157"/>
     </row>
     <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="36" t="s">
         <v>332</v>
       </c>
-      <c r="C60" s="145"/>
+      <c r="C60" s="146"/>
       <c r="D60" s="32" t="s">
         <v>341</v>
       </c>
@@ -16342,13 +16345,13 @@
       <c r="F60" s="32" t="s">
         <v>356</v>
       </c>
-      <c r="G60" s="142"/>
+      <c r="G60" s="158"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" s="37" t="s">
         <v>333</v>
       </c>
-      <c r="C61" s="151" t="s">
+      <c r="C61" s="149" t="s">
         <v>243</v>
       </c>
       <c r="D61" s="30" t="s">
@@ -16360,7 +16363,7 @@
       <c r="F61" s="30" t="s">
         <v>360</v>
       </c>
-      <c r="G61" s="140" t="s">
+      <c r="G61" s="156" t="s">
         <v>486</v>
       </c>
     </row>
@@ -16368,7 +16371,7 @@
       <c r="B62" s="37" t="s">
         <v>334</v>
       </c>
-      <c r="C62" s="152"/>
+      <c r="C62" s="150"/>
       <c r="D62" s="31" t="s">
         <v>343</v>
       </c>
@@ -16378,14 +16381,14 @@
       <c r="F62" s="31" t="s">
         <v>361</v>
       </c>
-      <c r="G62" s="141"/>
+      <c r="G62" s="157"/>
     </row>
     <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="23"/>
       <c r="B63" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="C63" s="153"/>
+      <c r="C63" s="151"/>
       <c r="D63" s="32" t="s">
         <v>344</v>
       </c>
@@ -16395,14 +16398,14 @@
       <c r="F63" s="32" t="s">
         <v>362</v>
       </c>
-      <c r="G63" s="142"/>
+      <c r="G63" s="158"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="23"/>
       <c r="B64" s="92" t="s">
         <v>363</v>
       </c>
-      <c r="C64" s="144" t="s">
+      <c r="C64" s="145" t="s">
         <v>244</v>
       </c>
       <c r="D64" s="30" t="s">
@@ -16414,7 +16417,7 @@
       <c r="F64" s="30" t="s">
         <v>390</v>
       </c>
-      <c r="G64" s="140" t="s">
+      <c r="G64" s="156" t="s">
         <v>481</v>
       </c>
     </row>
@@ -16422,7 +16425,7 @@
       <c r="B65" s="35" t="s">
         <v>364</v>
       </c>
-      <c r="C65" s="144"/>
+      <c r="C65" s="145"/>
       <c r="D65" s="31" t="s">
         <v>373</v>
       </c>
@@ -16432,13 +16435,13 @@
       <c r="F65" s="31" t="s">
         <v>391</v>
       </c>
-      <c r="G65" s="141"/>
+      <c r="G65" s="157"/>
     </row>
     <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="36" t="s">
         <v>365</v>
       </c>
-      <c r="C66" s="145"/>
+      <c r="C66" s="146"/>
       <c r="D66" s="95" t="s">
         <v>374</v>
       </c>
@@ -16448,13 +16451,13 @@
       <c r="F66" s="32" t="s">
         <v>392</v>
       </c>
-      <c r="G66" s="142"/>
+      <c r="G66" s="158"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B67" s="35" t="s">
         <v>366</v>
       </c>
-      <c r="C67" s="144" t="s">
+      <c r="C67" s="145" t="s">
         <v>245</v>
       </c>
       <c r="D67" s="30" t="s">
@@ -16466,7 +16469,7 @@
       <c r="F67" s="30" t="s">
         <v>393</v>
       </c>
-      <c r="G67" s="140" t="s">
+      <c r="G67" s="156" t="s">
         <v>481</v>
       </c>
     </row>
@@ -16474,7 +16477,7 @@
       <c r="B68" s="35" t="s">
         <v>367</v>
       </c>
-      <c r="C68" s="144"/>
+      <c r="C68" s="145"/>
       <c r="D68" s="31" t="s">
         <v>376</v>
       </c>
@@ -16484,13 +16487,13 @@
       <c r="F68" s="31" t="s">
         <v>394</v>
       </c>
-      <c r="G68" s="141"/>
+      <c r="G68" s="157"/>
     </row>
     <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="36" t="s">
         <v>368</v>
       </c>
-      <c r="C69" s="145"/>
+      <c r="C69" s="146"/>
       <c r="D69" s="32" t="s">
         <v>377</v>
       </c>
@@ -16500,13 +16503,13 @@
       <c r="F69" s="32" t="s">
         <v>395</v>
       </c>
-      <c r="G69" s="142"/>
+      <c r="G69" s="158"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B70" s="35" t="s">
         <v>369</v>
       </c>
-      <c r="C70" s="143" t="s">
+      <c r="C70" s="147" t="s">
         <v>246</v>
       </c>
       <c r="D70" s="30" t="s">
@@ -16518,7 +16521,7 @@
       <c r="F70" s="30" t="s">
         <v>396</v>
       </c>
-      <c r="G70" s="140" t="s">
+      <c r="G70" s="156" t="s">
         <v>486</v>
       </c>
     </row>
@@ -16527,7 +16530,7 @@
       <c r="B71" s="30" t="s">
         <v>370</v>
       </c>
-      <c r="C71" s="144"/>
+      <c r="C71" s="145"/>
       <c r="D71" s="31" t="s">
         <v>379</v>
       </c>
@@ -16537,14 +16540,14 @@
       <c r="F71" s="31" t="s">
         <v>397</v>
       </c>
-      <c r="G71" s="141"/>
+      <c r="G71" s="157"/>
     </row>
     <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="23"/>
       <c r="B72" s="36" t="s">
         <v>371</v>
       </c>
-      <c r="C72" s="145"/>
+      <c r="C72" s="146"/>
       <c r="D72" s="32" t="s">
         <v>380</v>
       </c>
@@ -16554,14 +16557,14 @@
       <c r="F72" s="32" t="s">
         <v>398</v>
       </c>
-      <c r="G72" s="142"/>
+      <c r="G72" s="158"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="23"/>
       <c r="B73" s="30" t="s">
         <v>399</v>
       </c>
-      <c r="C73" s="144" t="s">
+      <c r="C73" s="145" t="s">
         <v>247</v>
       </c>
       <c r="D73" s="30" t="s">
@@ -16573,7 +16576,7 @@
       <c r="F73" s="30" t="s">
         <v>422</v>
       </c>
-      <c r="G73" s="140" t="s">
+      <c r="G73" s="156" t="s">
         <v>481</v>
       </c>
     </row>
@@ -16582,7 +16585,7 @@
       <c r="B74" s="30" t="s">
         <v>400</v>
       </c>
-      <c r="C74" s="144"/>
+      <c r="C74" s="145"/>
       <c r="D74" s="31" t="s">
         <v>409</v>
       </c>
@@ -16592,14 +16595,14 @@
       <c r="F74" s="31" t="s">
         <v>423</v>
       </c>
-      <c r="G74" s="141"/>
+      <c r="G74" s="157"/>
     </row>
     <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="23"/>
       <c r="B75" s="32" t="s">
         <v>401</v>
       </c>
-      <c r="C75" s="145"/>
+      <c r="C75" s="146"/>
       <c r="D75" s="32" t="s">
         <v>410</v>
       </c>
@@ -16609,14 +16612,14 @@
       <c r="F75" s="32" t="s">
         <v>424</v>
       </c>
-      <c r="G75" s="142"/>
+      <c r="G75" s="158"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="23"/>
       <c r="B76" s="30" t="s">
         <v>402</v>
       </c>
-      <c r="C76" s="144" t="s">
+      <c r="C76" s="145" t="s">
         <v>248</v>
       </c>
       <c r="D76" s="30" t="s">
@@ -16628,7 +16631,7 @@
       <c r="F76" s="30" t="s">
         <v>543</v>
       </c>
-      <c r="G76" s="140" t="s">
+      <c r="G76" s="156" t="s">
         <v>487</v>
       </c>
     </row>
@@ -16637,7 +16640,7 @@
       <c r="B77" s="30" t="s">
         <v>403</v>
       </c>
-      <c r="C77" s="144"/>
+      <c r="C77" s="145"/>
       <c r="D77" s="94" t="s">
         <v>412</v>
       </c>
@@ -16647,14 +16650,14 @@
       <c r="F77" s="31" t="s">
         <v>544</v>
       </c>
-      <c r="G77" s="141"/>
+      <c r="G77" s="157"/>
     </row>
     <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="23"/>
       <c r="B78" s="32" t="s">
         <v>404</v>
       </c>
-      <c r="C78" s="145"/>
+      <c r="C78" s="146"/>
       <c r="D78" s="32" t="s">
         <v>441</v>
       </c>
@@ -16664,14 +16667,14 @@
       <c r="F78" s="32" t="s">
         <v>489</v>
       </c>
-      <c r="G78" s="142"/>
+      <c r="G78" s="158"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="23"/>
       <c r="B79" s="30" t="s">
         <v>405</v>
       </c>
-      <c r="C79" s="143" t="s">
+      <c r="C79" s="147" t="s">
         <v>249</v>
       </c>
       <c r="D79" s="30" t="s">
@@ -16683,7 +16686,7 @@
       <c r="F79" s="30" t="s">
         <v>425</v>
       </c>
-      <c r="G79" s="140" t="s">
+      <c r="G79" s="156" t="s">
         <v>486</v>
       </c>
     </row>
@@ -16692,7 +16695,7 @@
       <c r="B80" s="30" t="s">
         <v>406</v>
       </c>
-      <c r="C80" s="144"/>
+      <c r="C80" s="145"/>
       <c r="D80" s="31" t="s">
         <v>414</v>
       </c>
@@ -16702,14 +16705,14 @@
       <c r="F80" s="31" t="s">
         <v>426</v>
       </c>
-      <c r="G80" s="141"/>
+      <c r="G80" s="157"/>
     </row>
     <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="23"/>
       <c r="B81" s="32" t="s">
         <v>407</v>
       </c>
-      <c r="C81" s="145"/>
+      <c r="C81" s="146"/>
       <c r="D81" s="32" t="s">
         <v>415</v>
       </c>
@@ -16719,14 +16722,14 @@
       <c r="F81" s="32" t="s">
         <v>523</v>
       </c>
-      <c r="G81" s="142"/>
+      <c r="G81" s="158"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="23"/>
       <c r="B82" s="30" t="s">
         <v>427</v>
       </c>
-      <c r="C82" s="144" t="s">
+      <c r="C82" s="145" t="s">
         <v>250</v>
       </c>
       <c r="D82" s="30" t="s">
@@ -16738,7 +16741,7 @@
       <c r="F82" s="30" t="s">
         <v>455</v>
       </c>
-      <c r="G82" s="140" t="s">
+      <c r="G82" s="156" t="s">
         <v>486</v>
       </c>
     </row>
@@ -16747,7 +16750,7 @@
       <c r="B83" s="30" t="s">
         <v>428</v>
       </c>
-      <c r="C83" s="144"/>
+      <c r="C83" s="145"/>
       <c r="D83" s="94" t="s">
         <v>437</v>
       </c>
@@ -16757,14 +16760,14 @@
       <c r="F83" s="31" t="s">
         <v>456</v>
       </c>
-      <c r="G83" s="141"/>
+      <c r="G83" s="157"/>
     </row>
     <row r="84" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="23"/>
       <c r="B84" s="32" t="s">
         <v>429</v>
       </c>
-      <c r="C84" s="145"/>
+      <c r="C84" s="146"/>
       <c r="D84" s="95" t="s">
         <v>438</v>
       </c>
@@ -16774,14 +16777,14 @@
       <c r="F84" s="32" t="s">
         <v>457</v>
       </c>
-      <c r="G84" s="142"/>
+      <c r="G84" s="158"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="23"/>
       <c r="B85" s="30" t="s">
         <v>430</v>
       </c>
-      <c r="C85" s="144" t="s">
+      <c r="C85" s="145" t="s">
         <v>251</v>
       </c>
       <c r="D85" s="30" t="s">
@@ -16793,7 +16796,7 @@
       <c r="F85" s="30" t="s">
         <v>458</v>
       </c>
-      <c r="G85" s="140" t="s">
+      <c r="G85" s="156" t="s">
         <v>486</v>
       </c>
     </row>
@@ -16802,7 +16805,7 @@
       <c r="B86" s="30" t="s">
         <v>431</v>
       </c>
-      <c r="C86" s="144"/>
+      <c r="C86" s="145"/>
       <c r="D86" s="31" t="s">
         <v>440</v>
       </c>
@@ -16812,14 +16815,14 @@
       <c r="F86" s="31" t="s">
         <v>459</v>
       </c>
-      <c r="G86" s="141"/>
+      <c r="G86" s="157"/>
     </row>
     <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="23"/>
       <c r="B87" s="32" t="s">
         <v>432</v>
       </c>
-      <c r="C87" s="145"/>
+      <c r="C87" s="146"/>
       <c r="D87" s="32" t="s">
         <v>442</v>
       </c>
@@ -16829,14 +16832,14 @@
       <c r="F87" s="32" t="s">
         <v>460</v>
       </c>
-      <c r="G87" s="142"/>
+      <c r="G87" s="158"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="23"/>
       <c r="B88" s="30" t="s">
         <v>433</v>
       </c>
-      <c r="C88" s="143" t="s">
+      <c r="C88" s="147" t="s">
         <v>252</v>
       </c>
       <c r="D88" s="30" t="s">
@@ -16848,7 +16851,7 @@
       <c r="F88" s="30" t="s">
         <v>461</v>
       </c>
-      <c r="G88" s="140" t="s">
+      <c r="G88" s="156" t="s">
         <v>486</v>
       </c>
     </row>
@@ -16857,7 +16860,7 @@
       <c r="B89" s="30" t="s">
         <v>434</v>
       </c>
-      <c r="C89" s="144"/>
+      <c r="C89" s="145"/>
       <c r="D89" s="31" t="s">
         <v>444</v>
       </c>
@@ -16867,14 +16870,14 @@
       <c r="F89" s="31" t="s">
         <v>462</v>
       </c>
-      <c r="G89" s="141"/>
+      <c r="G89" s="157"/>
     </row>
     <row r="90" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="23"/>
       <c r="B90" s="32" t="s">
         <v>435</v>
       </c>
-      <c r="C90" s="145"/>
+      <c r="C90" s="146"/>
       <c r="D90" s="32" t="s">
         <v>445</v>
       </c>
@@ -16884,15 +16887,44 @@
       <c r="F90" s="32" t="s">
         <v>463</v>
       </c>
-      <c r="G90" s="142"/>
+      <c r="G90" s="158"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="C76:C78"/>
-    <mergeCell ref="C79:C81"/>
-    <mergeCell ref="C82:C84"/>
-    <mergeCell ref="C85:C87"/>
-    <mergeCell ref="C88:C90"/>
+    <mergeCell ref="G82:G84"/>
+    <mergeCell ref="G85:G87"/>
+    <mergeCell ref="G88:G90"/>
+    <mergeCell ref="G67:G69"/>
+    <mergeCell ref="G70:G72"/>
+    <mergeCell ref="G73:G75"/>
+    <mergeCell ref="G76:G78"/>
+    <mergeCell ref="G79:G81"/>
+    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="G55:G57"/>
+    <mergeCell ref="G58:G60"/>
+    <mergeCell ref="G61:G63"/>
+    <mergeCell ref="G64:G66"/>
+    <mergeCell ref="G37:G39"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="G49:G51"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="B34:D34"/>
     <mergeCell ref="C73:C75"/>
     <mergeCell ref="C40:C42"/>
     <mergeCell ref="C43:C45"/>
@@ -16905,40 +16937,11 @@
     <mergeCell ref="C64:C66"/>
     <mergeCell ref="C67:C69"/>
     <mergeCell ref="C70:C72"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="I17:I19"/>
-    <mergeCell ref="G37:G39"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="G43:G45"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="G49:G51"/>
-    <mergeCell ref="G52:G54"/>
-    <mergeCell ref="G55:G57"/>
-    <mergeCell ref="G58:G60"/>
-    <mergeCell ref="G61:G63"/>
-    <mergeCell ref="G64:G66"/>
-    <mergeCell ref="G82:G84"/>
-    <mergeCell ref="G85:G87"/>
-    <mergeCell ref="G88:G90"/>
-    <mergeCell ref="G67:G69"/>
-    <mergeCell ref="G70:G72"/>
-    <mergeCell ref="G73:G75"/>
-    <mergeCell ref="G76:G78"/>
-    <mergeCell ref="G79:G81"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="C82:C84"/>
+    <mergeCell ref="C85:C87"/>
+    <mergeCell ref="C88:C90"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -16994,8 +16997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{001D0DC7-188F-4907-92DF-1ADC13272703}">
   <dimension ref="B2:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17015,11 +17018,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="J2" s="123" t="s">
+      <c r="J2" s="128" t="s">
         <v>490</v>
       </c>
-      <c r="K2" s="123"/>
-      <c r="L2" s="123"/>
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
@@ -17579,7 +17582,7 @@
       <c r="C19" s="8">
         <v>111222666</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="121" t="s">
         <v>172</v>
       </c>
       <c r="E19" s="68" t="s">
@@ -17987,7 +17990,7 @@
     <hyperlink ref="C20" location="Organização!D9" display="Organização!D9" xr:uid="{68D45E4F-72C4-487A-9905-E683C105335B}"/>
     <hyperlink ref="D17" location="Organização!E40" display="tomas@marcelo.advogados.pt" xr:uid="{EC34DC22-193A-47F0-B2AE-41BB61DE744E}"/>
     <hyperlink ref="D18" location="Organização!E40" display="tomas@marcelo.advogados.pt" xr:uid="{DB1E40B0-83B9-4CDF-941F-109010250DEC}"/>
-    <hyperlink ref="D19" location="Organização!E39" display="francisca@marcelo.advogados.pt" xr:uid="{95489C89-A2D0-47B2-B01D-99361F24FBE0}"/>
+    <hyperlink ref="D19" r:id="rId1" xr:uid="{95489C89-A2D0-47B2-B01D-99361F24FBE0}"/>
     <hyperlink ref="D20" location="Organização!E39" display="francisca@marcelo.advogados.pt" xr:uid="{0464B481-CE53-4096-AA36-15A7FCA92E28}"/>
     <hyperlink ref="E17" location="AreaAtividade!D30" display="AC-006_01" xr:uid="{76E4DD76-27CB-4CF0-983D-70608F3E6124}"/>
     <hyperlink ref="E18" location="AreaAtividade!D30" display="AC-006_01" xr:uid="{634E9415-9D92-4488-9179-8362F9D203B1}"/>
@@ -18019,5 +18022,6 @@
     <hyperlink ref="E28" location="AreaAtividade!D24" display="AC-004_01" xr:uid="{9A1E3EE0-32D0-4584-90E1-C936CCDE7FDF}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>